<commit_message>
Begin the process of a design shrink
</commit_message>
<xml_diff>
--- a/Board/BOM.xlsx
+++ b/Board/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0xxxa\Desktop\Arduino-Thermostat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Arduino-Thermostat\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BEF067-E3BB-46F6-8FB0-49F3D6AC2040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF04CC84-8881-4B63-96DD-EB358431B542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,21 +69,12 @@
     <t>Capicitor 680uF</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/rubycon/50PX680MEFC12-5X20/3134365</t>
-  </si>
-  <si>
     <t>Inductor 53 uH</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/pulse-electronics-power/PE-54039NL/2266132</t>
-  </si>
-  <si>
     <t>Schottky Diode</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/smc-diode-solutions/SB5100TA/6022969</t>
-  </si>
-  <si>
     <t>Buttons</t>
   </si>
   <si>
@@ -102,9 +93,6 @@
     <t>https://www.digikey.com/en/products/detail/focus-lcds/C162A-BW-LW65/13901792</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-potter-brumfield-relays/PCH-105L2MH-000/2398819</t>
-  </si>
-  <si>
     <t>Pot</t>
   </si>
   <si>
@@ -115,6 +103,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/mdd/KBP307-L/14825026</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electric-works/DS1E-M-DC5V/280951</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/7447471101/3476776</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/smc-diode-solutions/31DQ05TA/12142429</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nichicon/UVY1J221MPD1TD/4328548</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +473,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,40 +517,40 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -599,35 +599,35 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added E-Ink Display files
Started making E-Ink Display footprints
</commit_message>
<xml_diff>
--- a/Board/BOM.xlsx
+++ b/Board/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Arduino-Thermostat\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8CA6CF-9B08-4B1F-8B87-BC924E25E7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE864F1-A25B-428A-A601-C76533718086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Description</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Capicitor 220uF</t>
+  </si>
+  <si>
+    <t>e-Ink Display</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/4777</t>
   </si>
 </sst>
 </file>
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +634,17 @@
       </c>
       <c r="C16" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued E-Ink display transition
</commit_message>
<xml_diff>
--- a/Board/BOM.xlsx
+++ b/Board/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Arduino-Thermostat\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE864F1-A25B-428A-A601-C76533718086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD221F68-801F-4D8F-B2FD-0BCE41EA1A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Description</t>
   </si>
@@ -39,9 +40,6 @@
     <t>Relay</t>
   </si>
   <si>
-    <t>Relay Driver</t>
-  </si>
-  <si>
     <t>2 Position Screw Terminal</t>
   </si>
   <si>
@@ -57,57 +55,21 @@
     <t>Sourced Locally</t>
   </si>
   <si>
-    <t>Arduino Nano</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/L293D/634700</t>
-  </si>
-  <si>
     <t>Voltage Regulator</t>
   </si>
   <si>
-    <t>Inductor 53 uH</t>
-  </si>
-  <si>
     <t>Schottky Diode</t>
   </si>
   <si>
-    <t>Buttons</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/apem-inc/MJTP1230/1798037</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/phoenix-contact/5442206/4390264</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM2596T-5-0-NOPB/363708</t>
-  </si>
-  <si>
-    <t>LCD Display</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/focus-lcds/C162A-BW-LW65/13901792</t>
-  </si>
-  <si>
-    <t>Pot</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/bourns-inc/PV36W103C01B00/666502</t>
-  </si>
-  <si>
     <t>Rectifier</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/mdd/KBP307-L/14825026</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/panasonic-electric-works/DS1E-M-DC5V/280951</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/7447471101/3476776</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/smc-diode-solutions/31DQ05TA/12142429</t>
   </si>
   <si>
@@ -121,6 +83,18 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/4777</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electric-works/DS1E-M-DC3V/647259</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM2596S-3-3/3701219</t>
+  </si>
+  <si>
+    <t>Inductor 68 uH</t>
+  </si>
+  <si>
+    <t>MCU</t>
   </si>
 </sst>
 </file>
@@ -449,15 +423,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="117" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -479,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -487,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -495,171 +470,116 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
+      <c r="C8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
+      <c r="C9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
+      <c r="C15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1" xr:uid="{BF465262-A6E5-4B4F-ABDA-2F83F19B9E4D}"/>
-    <hyperlink ref="C6" r:id="rId2" xr:uid="{A5F5E8AA-D6BE-420C-8D67-0F60F658C6A6}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{D146D22B-32CB-4D73-BFA5-370C866ABEEE}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{8C9EB3AC-5791-48B8-875A-8A129F578389}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{9A932A9A-5EE4-4CCB-BF8E-BE97718A3E58}"/>
-    <hyperlink ref="C9" r:id="rId6" xr:uid="{5D0EA190-0990-44BD-803C-690FE7DEE362}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{1DD29441-5278-4476-8E24-41C17C67DC49}"/>
-    <hyperlink ref="C14" r:id="rId8" xr:uid="{F03B2194-6067-4252-82E8-3ECB6948AD7B}"/>
-    <hyperlink ref="C15" r:id="rId9" xr:uid="{FA084577-B508-4D1F-A442-985C6DE067E8}"/>
-    <hyperlink ref="C16" r:id="rId10" xr:uid="{6B729F37-69ED-433C-B034-22B0145AD91D}"/>
-    <hyperlink ref="C2" r:id="rId11" xr:uid="{839FB170-B563-49EE-BF33-DF83C93FF05B}"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{BF465262-A6E5-4B4F-ABDA-2F83F19B9E4D}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{A5F5E8AA-D6BE-420C-8D67-0F60F658C6A6}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{8C9EB3AC-5791-48B8-875A-8A129F578389}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{6B729F37-69ED-433C-B034-22B0145AD91D}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{37F912BD-81A6-499D-9729-1571600601B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finish Schematic for new PCB
</commit_message>
<xml_diff>
--- a/Board/BOM.xlsx
+++ b/Board/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Arduino-Thermostat\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD221F68-801F-4D8F-B2FD-0BCE41EA1A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70A6DA7-E7B6-4E7C-99E8-9524FD4BE5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -95,6 +94,15 @@
   </si>
   <si>
     <t>MCU</t>
+  </si>
+  <si>
+    <t>Logic Level FET</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/infineon-technologies/BSS806NH6327XTSA1/2783472</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/2211-H-RC/775363</t>
   </si>
 </sst>
 </file>
@@ -426,7 +434,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +516,9 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -552,6 +562,17 @@
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished board layout, updated readme
</commit_message>
<xml_diff>
--- a/Board/BOM.xlsx
+++ b/Board/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Arduino-Thermostat\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8933C12-AAB9-472A-B874-AE78CD29A55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDE1DA8-A829-40F3-B148-ACCB740F39E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Description</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/panasonic-electric-works/DS1E-S-DC3V/413288</t>
+  </si>
+  <si>
+    <t>Fuse Holder</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/keystone-electronics/3568/2137306</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/eaton-bussmann-electrical-division/BK-ATM-3/264847</t>
   </si>
 </sst>
 </file>
@@ -573,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,6 +815,28 @@
       </c>
       <c r="C20" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started E-Ink interface programming
</commit_message>
<xml_diff>
--- a/Board/BOM.xlsx
+++ b/Board/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Arduino-Thermostat\Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDE1DA8-A829-40F3-B148-ACCB740F39E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA44610-C213-443A-A420-C4EB80F7F24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,10 +198,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -588,7 +589,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +616,7 @@
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -637,7 +638,7 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -736,7 +737,7 @@
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -747,7 +748,7 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -758,7 +759,7 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -791,7 +792,7 @@
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -802,7 +803,7 @@
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -813,7 +814,7 @@
       <c r="B20">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -824,7 +825,7 @@
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -835,7 +836,7 @@
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -847,6 +848,16 @@
     <hyperlink ref="C7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="C11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="C12" r:id="rId6" xr:uid="{AE4277EE-4684-4E86-B2AE-0115DDBF1633}"/>
+    <hyperlink ref="C2" r:id="rId7" xr:uid="{CFFDBA73-3F94-41B0-B9BA-1BEDC3ECD7ED}"/>
+    <hyperlink ref="C4" r:id="rId8" xr:uid="{A1491D64-B01C-41D8-A30A-6CCFDEF9787B}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{3D2F4571-A75F-43F4-975A-DE7A330944D4}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{1FA7D09A-1EF4-4794-8AEF-1289939CB4FD}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{6F2DD68A-EDBF-4D19-B07C-A48FC023CC1B}"/>
+    <hyperlink ref="C18" r:id="rId12" xr:uid="{18D18F6E-F4AE-474B-8AE7-4E47E50628B7}"/>
+    <hyperlink ref="C19" r:id="rId13" xr:uid="{24D2A23F-5B2F-4F22-95F9-941B59C19667}"/>
+    <hyperlink ref="C20" r:id="rId14" xr:uid="{B77CC612-9513-4F69-AADF-B0EE0A84AD0A}"/>
+    <hyperlink ref="C21" r:id="rId15" xr:uid="{6ED3FA1F-6A27-41DE-8B5D-EC3C25F7D519}"/>
+    <hyperlink ref="C22" r:id="rId16" xr:uid="{B11543BE-0AFB-49FB-B92A-7F5104FFABDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>